<commit_message>
database: update minoxd sheet
</commit_message>
<xml_diff>
--- a/DataBase_For_Facebook.xlsx
+++ b/DataBase_For_Facebook.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\FaceBook_Backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\mino-usth\B3\FaceBook_Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C1017F-3376-4643-A966-872C9D9C5BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A17B52-C3D4-4EF3-9D91-DA3F4180BAC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="126">
   <si>
     <t>Column1</t>
   </si>
@@ -343,13 +344,82 @@
   </si>
   <si>
     <t>In-Processing</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>category_id</t>
+  </si>
+  <si>
+    <t>owned_by</t>
+  </si>
+  <si>
+    <t>avatar_url</t>
+  </si>
+  <si>
+    <t>background_url</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>instagram</t>
+  </si>
+  <si>
+    <t>Page_Category</t>
+  </si>
+  <si>
+    <t>Page_Follower</t>
+  </si>
+  <si>
+    <t>page_id</t>
+  </si>
+  <si>
+    <t>liked</t>
+  </si>
+  <si>
+    <t>followed</t>
+  </si>
+  <si>
+    <t>Photo_Tag</t>
+  </si>
+  <si>
+    <t>tagged_user_id</t>
+  </si>
+  <si>
+    <t>Album</t>
+  </si>
+  <si>
+    <t>Album_Photo</t>
+  </si>
+  <si>
+    <t>album_id</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>type_id</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>Event_Type</t>
+  </si>
+  <si>
+    <t>Item_Category</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -402,6 +472,13 @@
     <font>
       <sz val="9.8000000000000007"/>
       <name val="JetBrains Mono"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -469,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -484,6 +561,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -503,9 +587,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -543,7 +627,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -649,7 +733,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -791,7 +875,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -804,21 +888,21 @@
   </sheetPr>
   <dimension ref="A2:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="15" max="15" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" thickBot="1">
@@ -868,7 +952,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:15" thickTop="1">
+    <row r="3" spans="1:15" ht="15" thickTop="1">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -904,7 +988,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15">
+    <row r="4" spans="1:15" ht="14.4">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -927,7 +1011,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15">
+    <row r="5" spans="1:15" ht="14.4">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -959,7 +1043,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15">
+    <row r="6" spans="1:15" ht="14.4">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -988,7 +1072,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15">
+    <row r="7" spans="1:15" ht="14.4">
       <c r="A7" s="2" t="s">
         <v>91</v>
       </c>
@@ -1014,7 +1098,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15">
+    <row r="8" spans="1:15" ht="14.4">
       <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
@@ -1055,7 +1139,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15">
+    <row r="9" spans="1:15" ht="14.4">
       <c r="A9" s="2" t="s">
         <v>38</v>
       </c>
@@ -1093,7 +1177,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15">
+    <row r="10" spans="1:15" ht="14.4">
       <c r="A10" s="2" t="s">
         <v>90</v>
       </c>
@@ -1659,4 +1743,1078 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A405F1-D02F-4C21-B112-0CBEF8B49B93}">
+  <dimension ref="A2:O31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="13.2"/>
+  <cols>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" customWidth="1"/>
+    <col min="15" max="15" width="16.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:15" ht="13.8" thickBot="1">
+      <c r="A2" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="13.8" thickTop="1">
+      <c r="A3" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A16" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A17" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A18" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+    </row>
+    <row r="19" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A22" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="M22" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A24" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L24" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="M24" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="5" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A26" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A27" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A28" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A29" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A30" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A31" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="Hãy lựa chọn Quá Trình" sqref="O3:O31 A3:A31" xr:uid="{CCD98658-CC92-4705-9AB1-EE80A89EBFA1}">
+      <formula1>"Done!, Not Done!, In-Processing, None"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: add fields for entities (avatarUrl for user, name for page
</commit_message>
<xml_diff>
--- a/DataBase_For_Facebook.xlsx
+++ b/DataBase_For_Facebook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\mino-usth\B3\FaceBook_Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A17B52-C3D4-4EF3-9D91-DA3F4180BAC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1993F559-808F-4A4B-95E0-0EAEA4851FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="127">
   <si>
     <t>Column1</t>
   </si>
@@ -413,6 +413,9 @@
   </si>
   <si>
     <t>Item_Category</t>
+  </si>
+  <si>
+    <t>avatarUrl</t>
   </si>
 </sst>
 </file>
@@ -1750,7 +1753,7 @@
   <dimension ref="A2:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="13.2"/>
@@ -1844,7 +1847,9 @@
       <c r="J3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="5"/>
+      <c r="K3" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="L3" s="5"/>
       <c r="M3" s="4"/>
       <c r="N3" s="5"/>
@@ -2190,30 +2195,32 @@
         <v>30</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="J13" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="K13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="L13" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="L13" s="5"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5" t="s">

</xml_diff>